<commit_message>
modify NL excel file
Signed-off-by: Nitish Bharambe <nitish.bharambe@alliander.com>
</commit_message>
<xml_diff>
--- a/tests/data/vision/vision_nl.xlsx
+++ b/tests/data/vision/vision_nl.xlsx
@@ -8,29 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alliander-my.sharepoint.com/personal/nitish_bharambe_alliander_com/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF4A3D4A-256C-446C-B77B-ABE11994FF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31F811ED-4E9F-4BBC-8DC9-FC1285BC215F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nodes" sheetId="2" r:id="rId1"/>
-    <sheet name="Cable parts" sheetId="3" r:id="rId2"/>
-    <sheet name="Cables" sheetId="4" r:id="rId3"/>
-    <sheet name="Lines" sheetId="5" r:id="rId4"/>
+    <sheet name="Knooppunten" sheetId="2" r:id="rId1"/>
+    <sheet name="Kabeldelen" sheetId="3" r:id="rId2"/>
+    <sheet name="Kabels" sheetId="4" r:id="rId3"/>
+    <sheet name="Verbindingen" sheetId="5" r:id="rId4"/>
     <sheet name="Links" sheetId="6" r:id="rId5"/>
-    <sheet name="Reactance coils" sheetId="7" r:id="rId6"/>
-    <sheet name="Transformers" sheetId="8" r:id="rId7"/>
-    <sheet name="Special transformers" sheetId="9" r:id="rId8"/>
-    <sheet name="Three winding transformers" sheetId="10" r:id="rId9"/>
-    <sheet name="Sources" sheetId="11" r:id="rId10"/>
-    <sheet name="Synchronous generators" sheetId="12" r:id="rId11"/>
-    <sheet name="Wind turbines" sheetId="13" r:id="rId12"/>
-    <sheet name="Loads" sheetId="14" r:id="rId13"/>
-    <sheet name="Transformer loads" sheetId="15" r:id="rId14"/>
-    <sheet name="Capacitors" sheetId="16" r:id="rId15"/>
-    <sheet name="Reactors" sheetId="17" r:id="rId16"/>
-    <sheet name="Zigzag transformers" sheetId="18" r:id="rId17"/>
-    <sheet name="Pvs" sheetId="19" r:id="rId18"/>
+    <sheet name="Smoorspoelen" sheetId="7" r:id="rId6"/>
+    <sheet name="Transformatoren" sheetId="8" r:id="rId7"/>
+    <sheet name="Speciale transformatoren" sheetId="9" r:id="rId8"/>
+    <sheet name="Driewikkelingstransformatoren" sheetId="10" r:id="rId9"/>
+    <sheet name="Netvoedingen" sheetId="11" r:id="rId10"/>
+    <sheet name="Synchrone generatoren" sheetId="12" r:id="rId11"/>
+    <sheet name="Windturbines" sheetId="13" r:id="rId12"/>
+    <sheet name="Belastingen" sheetId="14" r:id="rId13"/>
+    <sheet name="Transformatorbelastingen" sheetId="15" r:id="rId14"/>
+    <sheet name="Condensatoren" sheetId="16" r:id="rId15"/>
+    <sheet name="Spoelen" sheetId="17" r:id="rId16"/>
+    <sheet name="Nulpuntstransformatoren" sheetId="18" r:id="rId17"/>
+    <sheet name="Pv's" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -39,13 +39,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="303">
   <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Short name</t>
+    <t>Nummer</t>
+  </si>
+  <si>
+    <t>Naam</t>
+  </si>
+  <si>
+    <t>Korte naam</t>
   </si>
   <si>
     <t>ID</t>
@@ -57,16 +57,16 @@
     <t>kV</t>
   </si>
   <si>
-    <t>Simultaneity</t>
-  </si>
-  <si>
-    <t>Busbar system</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Bad reachable</t>
+    <t>Gelijktijdigheid</t>
+  </si>
+  <si>
+    <t>Railsysteem</t>
+  </si>
+  <si>
+    <t>Functie</t>
+  </si>
+  <si>
+    <t>Slecht bereikbaar</t>
   </si>
   <si>
     <t>GX</t>
@@ -75,34 +75,34 @@
     <t>GY</t>
   </si>
   <si>
-    <t>Failure frequency</t>
-  </si>
-  <si>
-    <t>/year</t>
-  </si>
-  <si>
-    <t>Repair duration</t>
+    <t>Faalfrequentie</t>
+  </si>
+  <si>
+    <t>/jaar</t>
+  </si>
+  <si>
+    <t>Reparatieduur</t>
   </si>
   <si>
     <t>min</t>
   </si>
   <si>
-    <t>Maintenance frequency</t>
-  </si>
-  <si>
-    <t>Maintenance duration</t>
-  </si>
-  <si>
-    <t>Maint. cut-off duration</t>
-  </si>
-  <si>
-    <t>Remotely indicated status</t>
-  </si>
-  <si>
-    <t>Rail type</t>
-  </si>
-  <si>
-    <t>Rail type.Unom</t>
+    <t>Onderhoudsfrequentie</t>
+  </si>
+  <si>
+    <t>Onderhoudsduur</t>
+  </si>
+  <si>
+    <t>Onderhoudsafbreekduur</t>
+  </si>
+  <si>
+    <t>Verrestatus</t>
+  </si>
+  <si>
+    <t>Railtype</t>
+  </si>
+  <si>
+    <t>Railtype.Unom</t>
   </si>
   <si>
     <t>Inom</t>
@@ -111,49 +111,49 @@
     <t>A</t>
   </si>
   <si>
-    <t>Ik,dynamic</t>
+    <t>Ik,dynamisch</t>
   </si>
   <si>
     <t>kA</t>
   </si>
   <si>
-    <t>Ik,thermal</t>
-  </si>
-  <si>
-    <t>t,thermal</t>
+    <t>Ik,thermisch</t>
+  </si>
+  <si>
+    <t>t,thermisch</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
-    <t>RC frequency</t>
+    <t>TF-frequentie</t>
   </si>
   <si>
     <t>Hz</t>
   </si>
   <si>
-    <t>RC voltage</t>
+    <t>TF-spanning</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>TF angle</t>
+    <t>TF-hoek</t>
   </si>
   <si>
     <t>·</t>
   </si>
   <si>
-    <t>Re</t>
+    <t>Ra</t>
   </si>
   <si>
     <t>Ohm</t>
   </si>
   <si>
-    <t>Xe</t>
-  </si>
-  <si>
-    <t>Fields</t>
+    <t>Xa</t>
+  </si>
+  <si>
+    <t>Velden</t>
   </si>
   <si>
     <t>node1</t>
@@ -168,34 +168,34 @@
     <t>node4</t>
   </si>
   <si>
-    <t>Cable.Number</t>
-  </si>
-  <si>
-    <t>Cable.Name</t>
-  </si>
-  <si>
-    <t>Order number</t>
+    <t>Kabel.Nummer</t>
+  </si>
+  <si>
+    <t>Kabel.Naam</t>
+  </si>
+  <si>
+    <t>Volgnummer</t>
   </si>
   <si>
     <t>#Parallel</t>
   </si>
   <si>
-    <t>Cable type</t>
-  </si>
-  <si>
-    <t>Type short</t>
-  </si>
-  <si>
-    <t>Length</t>
+    <t>Kabeltype</t>
+  </si>
+  <si>
+    <t>Type kort</t>
+  </si>
+  <si>
+    <t>Lengte</t>
   </si>
   <si>
     <t>m</t>
   </si>
   <si>
-    <t>Ampacity factor</t>
-  </si>
-  <si>
-    <t>Year</t>
+    <t>Belastbaarheidsfactor</t>
+  </si>
+  <si>
+    <t>Jaar</t>
   </si>
   <si>
     <t>G</t>
@@ -204,7 +204,7 @@
     <t>Km/W</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>Prijs</t>
   </si>
   <si>
     <t>$/m</t>
@@ -246,10 +246,10 @@
     <t>TIk (1s)</t>
   </si>
   <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Pulse velocity</t>
+    <t>Frequentie</t>
+  </si>
+  <si>
+    <t>Loopsnelheid</t>
   </si>
   <si>
     <t>m/µs</t>
@@ -264,37 +264,37 @@
     <t>240 Al X</t>
   </si>
   <si>
-    <t>From.Number</t>
-  </si>
-  <si>
-    <t>From.Name</t>
-  </si>
-  <si>
-    <t>From.ID</t>
-  </si>
-  <si>
-    <t>From.Field</t>
-  </si>
-  <si>
-    <t>From.Switch state</t>
-  </si>
-  <si>
-    <t>To.Number</t>
-  </si>
-  <si>
-    <t>To.Name</t>
-  </si>
-  <si>
-    <t>To.ID</t>
-  </si>
-  <si>
-    <t>To.Field</t>
-  </si>
-  <si>
-    <t>To.Switch state</t>
-  </si>
-  <si>
-    <t>/km/year</t>
+    <t>Van.Nummer</t>
+  </si>
+  <si>
+    <t>Van.Naam</t>
+  </si>
+  <si>
+    <t>Van.ID</t>
+  </si>
+  <si>
+    <t>Van.Veld</t>
+  </si>
+  <si>
+    <t>Van.Schakelstand</t>
+  </si>
+  <si>
+    <t>Naar.Nummer</t>
+  </si>
+  <si>
+    <t>Naar.Naam</t>
+  </si>
+  <si>
+    <t>Naar.ID</t>
+  </si>
+  <si>
+    <t>Naar.Veld</t>
+  </si>
+  <si>
+    <t>Naar.Schakelstand</t>
+  </si>
+  <si>
+    <t>/km/jaar</t>
   </si>
   <si>
     <t>Inom'</t>
@@ -306,19 +306,19 @@
     <t>$</t>
   </si>
   <si>
-    <t>#Cable parts</t>
-  </si>
-  <si>
-    <t>#Joints</t>
-  </si>
-  <si>
-    <t>Joint failure frequency</t>
+    <t>#Kabeldelen</t>
+  </si>
+  <si>
+    <t>#Moffen</t>
+  </si>
+  <si>
+    <t>Moffaalfrequentie</t>
   </si>
   <si>
     <t>in</t>
   </si>
   <si>
-    <t>#Line parts</t>
+    <t>#Verbindingdelen</t>
   </si>
   <si>
     <t>line1</t>
@@ -348,7 +348,7 @@
     <t>0.3 Ohm</t>
   </si>
   <si>
-    <t>Tap</t>
+    <t>Trapstand</t>
   </si>
   <si>
     <t>Step up</t>
@@ -357,19 +357,19 @@
     <t>N1</t>
   </si>
   <si>
-    <t>Re1</t>
-  </si>
-  <si>
-    <t>Xe1</t>
+    <t>Ra1</t>
+  </si>
+  <si>
+    <t>Xa1</t>
   </si>
   <si>
     <t>N2</t>
   </si>
   <si>
-    <t>Re2</t>
-  </si>
-  <si>
-    <t>Xe2</t>
+    <t>Ra2</t>
+  </si>
+  <si>
+    <t>Xa2</t>
   </si>
   <si>
     <t>Snom'</t>
@@ -378,16 +378,16 @@
     <t>MVA</t>
   </si>
   <si>
-    <t>Phase shift</t>
+    <t>Fasedraaiing</t>
   </si>
   <si>
     <t>Graden</t>
   </si>
   <si>
-    <t>Measuring side</t>
-  </si>
-  <si>
-    <t>Control</t>
+    <t>Meetzijde</t>
+  </si>
+  <si>
+    <t>Regeling</t>
   </si>
   <si>
     <t>Uset</t>
@@ -426,40 +426,40 @@
     <t>kW</t>
   </si>
   <si>
-    <t>Po</t>
-  </si>
-  <si>
-    <t>Io</t>
+    <t>Pnul</t>
+  </si>
+  <si>
+    <t>Inul</t>
   </si>
   <si>
     <t>Z0</t>
   </si>
   <si>
-    <t>Connection</t>
-  </si>
-  <si>
-    <t>Tap side</t>
-  </si>
-  <si>
-    <t>Tap size</t>
-  </si>
-  <si>
-    <t>Tap min</t>
-  </si>
-  <si>
-    <t>Tap nom</t>
-  </si>
-  <si>
-    <t>Tap max</t>
+    <t>Schakeling</t>
+  </si>
+  <si>
+    <t>Trapzijde</t>
+  </si>
+  <si>
+    <t>Trapgrootte</t>
+  </si>
+  <si>
+    <t>Trapmin</t>
+  </si>
+  <si>
+    <t>Trapnom</t>
+  </si>
+  <si>
+    <t>Trapmax</t>
   </si>
   <si>
     <t>transformer1</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>own</t>
+    <t>geen</t>
+  </si>
+  <si>
+    <t>eigen</t>
   </si>
   <si>
     <t>10750/420 V  630 kVA</t>
@@ -471,7 +471,7 @@
     <t>Dyn5</t>
   </si>
   <si>
-    <t>Sort</t>
+    <t>Soort</t>
   </si>
   <si>
     <t>ukmin</t>
@@ -504,64 +504,64 @@
     <t>23 MVA</t>
   </si>
   <si>
-    <t>Node1.Number</t>
-  </si>
-  <si>
-    <t>Node1.Name</t>
-  </si>
-  <si>
-    <t>Node1.ID</t>
-  </si>
-  <si>
-    <t>Node1.Field</t>
-  </si>
-  <si>
-    <t>Switch state 1</t>
-  </si>
-  <si>
-    <t>Node2.Number</t>
-  </si>
-  <si>
-    <t>Node2.Name</t>
-  </si>
-  <si>
-    <t>Node2.ID</t>
-  </si>
-  <si>
-    <t>Node2.Field</t>
-  </si>
-  <si>
-    <t>Switch state 2</t>
-  </si>
-  <si>
-    <t>Node3.Number</t>
-  </si>
-  <si>
-    <t>Node3.Name</t>
-  </si>
-  <si>
-    <t>Node3.ID</t>
-  </si>
-  <si>
-    <t>Node3.Field</t>
-  </si>
-  <si>
-    <t>Switch state 3</t>
-  </si>
-  <si>
-    <t>Tap c</t>
-  </si>
-  <si>
-    <t>Tap a</t>
+    <t>Knooppunt1.Nummer</t>
+  </si>
+  <si>
+    <t>Knooppunt1.Naam</t>
+  </si>
+  <si>
+    <t>Knooppunt1.ID</t>
+  </si>
+  <si>
+    <t>Knooppunt1.Veld</t>
+  </si>
+  <si>
+    <t>Schakelstand1</t>
+  </si>
+  <si>
+    <t>Knooppunt2.Nummer</t>
+  </si>
+  <si>
+    <t>Knooppunt2.Naam</t>
+  </si>
+  <si>
+    <t>Knooppunt2.ID</t>
+  </si>
+  <si>
+    <t>Knooppunt2.Veld</t>
+  </si>
+  <si>
+    <t>Schakelstand2</t>
+  </si>
+  <si>
+    <t>Knooppunt3.Nummer</t>
+  </si>
+  <si>
+    <t>Knooppunt3.Naam</t>
+  </si>
+  <si>
+    <t>Knooppunt3.ID</t>
+  </si>
+  <si>
+    <t>Knooppunt3.Veld</t>
+  </si>
+  <si>
+    <t>Schakelstand3</t>
+  </si>
+  <si>
+    <t>Trapstand u</t>
+  </si>
+  <si>
+    <t>Trapstand i</t>
   </si>
   <si>
     <t>N3</t>
   </si>
   <si>
-    <t>Re3</t>
-  </si>
-  <si>
-    <t>Xe3</t>
+    <t>Ra3</t>
+  </si>
+  <si>
+    <t>Xa3</t>
   </si>
   <si>
     <t>Snom1'</t>
@@ -573,10 +573,10 @@
     <t>Snom3'</t>
   </si>
   <si>
-    <t>Phase shift 12</t>
-  </si>
-  <si>
-    <t>Phase shift 13</t>
+    <t>Fasedraaiing12</t>
+  </si>
+  <si>
+    <t>Fasedraaiing13</t>
   </si>
   <si>
     <t>Snom1</t>
@@ -609,13 +609,13 @@
     <t>Pk23</t>
   </si>
   <si>
-    <t>Sat12</t>
-  </si>
-  <si>
-    <t>Sat13</t>
-  </si>
-  <si>
-    <t>Sat23</t>
+    <t>Sbij12</t>
+  </si>
+  <si>
+    <t>Sbij13</t>
+  </si>
+  <si>
+    <t>Sbij23</t>
   </si>
   <si>
     <t>R012</t>
@@ -645,55 +645,55 @@
     <t>Ik(2s)3</t>
   </si>
   <si>
-    <t>Tap side c</t>
-  </si>
-  <si>
-    <t>Tap size c</t>
-  </si>
-  <si>
-    <t>Tap min c</t>
-  </si>
-  <si>
-    <t>Tap nom c</t>
-  </si>
-  <si>
-    <t>Tap max c</t>
-  </si>
-  <si>
-    <t>Tap side a</t>
-  </si>
-  <si>
-    <t>Tap size a</t>
-  </si>
-  <si>
-    <t>Tap min a</t>
-  </si>
-  <si>
-    <t>Tap nom a</t>
-  </si>
-  <si>
-    <t>Tap max a</t>
+    <t>Trapzijde u</t>
+  </si>
+  <si>
+    <t>Trapgrootte u</t>
+  </si>
+  <si>
+    <t>Trapmin u</t>
+  </si>
+  <si>
+    <t>Trapnom u</t>
+  </si>
+  <si>
+    <t>Trapmax u</t>
+  </si>
+  <si>
+    <t>Trapzijde i</t>
+  </si>
+  <si>
+    <t>Trapgrootte i</t>
+  </si>
+  <si>
+    <t>Trapmin i</t>
+  </si>
+  <si>
+    <t>Trapnom i</t>
+  </si>
+  <si>
+    <t>Trapmax i</t>
   </si>
   <si>
     <t>Dyn5yn7</t>
   </si>
   <si>
-    <t>Subnumber</t>
-  </si>
-  <si>
-    <t>Node.Number</t>
-  </si>
-  <si>
-    <t>Node.Name</t>
-  </si>
-  <si>
-    <t>Node.ID</t>
-  </si>
-  <si>
-    <t>Feeder</t>
-  </si>
-  <si>
-    <t>Switch state</t>
+    <t>Subnummer</t>
+  </si>
+  <si>
+    <t>Knooppunt.Nummer</t>
+  </si>
+  <si>
+    <t>Knooppunt.Naam</t>
+  </si>
+  <si>
+    <t>Knooppunt.ID</t>
+  </si>
+  <si>
+    <t>Veld</t>
+  </si>
+  <si>
+    <t>Schakelstand</t>
   </si>
   <si>
     <t>Uref</t>
@@ -702,7 +702,7 @@
     <t>pu</t>
   </si>
   <si>
-    <t>Angle</t>
+    <t>Hoek</t>
   </si>
   <si>
     <t>Sk"nom</t>
@@ -720,7 +720,7 @@
     <t>Z0/Z1</t>
   </si>
   <si>
-    <t>Profile</t>
+    <t>Profiel</t>
   </si>
   <si>
     <t>source1</t>
@@ -729,7 +729,7 @@
     <t>Default</t>
   </si>
   <si>
-    <t>Not preferent</t>
+    <t>Niet-preferent</t>
   </si>
   <si>
     <t>Pref</t>
@@ -738,10 +738,10 @@
     <t>MW</t>
   </si>
   <si>
-    <t>f/P droop</t>
-  </si>
-  <si>
-    <t>U/Q droop</t>
+    <t>f/P-statiek</t>
+  </si>
+  <si>
+    <t>U/Q-statiek</t>
   </si>
   <si>
     <t>cos phi</t>
@@ -771,7 +771,7 @@
     <t>xd"sat</t>
   </si>
   <si>
-    <t>Excitation</t>
+    <t>Bekrachtiging</t>
   </si>
   <si>
     <t>Rotor</t>
@@ -789,13 +789,13 @@
     <t>syngen1</t>
   </si>
   <si>
-    <t>cosine phi</t>
-  </si>
-  <si>
-    <t>supply</t>
-  </si>
-  <si>
-    <t>Wind speed</t>
+    <t>cosinus phi</t>
+  </si>
+  <si>
+    <t>leveren</t>
+  </si>
+  <si>
+    <t>Windsnelheid</t>
   </si>
   <si>
     <t>m/s</t>
@@ -804,10 +804,10 @@
     <t>Pnom</t>
   </si>
   <si>
-    <t>P control</t>
-  </si>
-  <si>
-    <t>Q control</t>
+    <t>P-regeling</t>
+  </si>
+  <si>
+    <t>Q-regeling</t>
   </si>
   <si>
     <t>wind1</t>
@@ -816,19 +816,19 @@
     <t>Async/75 kVA/0.4 kV</t>
   </si>
   <si>
-    <t>Fixed cos phi</t>
+    <t>Vaste cos phi</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
-    <t>Behaviour</t>
-  </si>
-  <si>
-    <t>Growth</t>
-  </si>
-  <si>
-    <t>Unbalanced</t>
+    <t>Gedrag</t>
+  </si>
+  <si>
+    <t>Groei</t>
+  </si>
+  <si>
+    <t>Asymmetrisch</t>
   </si>
   <si>
     <t>p123</t>
@@ -837,40 +837,40 @@
     <t>q123</t>
   </si>
   <si>
-    <t>#Large customers</t>
-  </si>
-  <si>
-    <t>#Generous customers</t>
-  </si>
-  <si>
-    <t>#Small customers</t>
-  </si>
-  <si>
-    <t>Harmonic type</t>
+    <t>#Grootverbruikers</t>
+  </si>
+  <si>
+    <t>#Royaalverbruikers</t>
+  </si>
+  <si>
+    <t>#Kleinverbruikers</t>
+  </si>
+  <si>
+    <t>Harmonischentype</t>
   </si>
   <si>
     <t>load1</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Load.P</t>
-  </si>
-  <si>
-    <t>Load.Q</t>
-  </si>
-  <si>
-    <t>Load.Profile</t>
-  </si>
-  <si>
-    <t>Generation.P</t>
-  </si>
-  <si>
-    <t>Generation.Q</t>
-  </si>
-  <si>
-    <t>Generation.Profile</t>
+    <t>Geen</t>
+  </si>
+  <si>
+    <t>Belasting.P</t>
+  </si>
+  <si>
+    <t>Belasting.Q</t>
+  </si>
+  <si>
+    <t>Belasting.Profiel</t>
+  </si>
+  <si>
+    <t>Opwekking.P</t>
+  </si>
+  <si>
+    <t>Opwekking.Q</t>
+  </si>
+  <si>
+    <t>Opwekking.Profiel</t>
   </si>
   <si>
     <t>PV.Pnom</t>
@@ -879,28 +879,28 @@
     <t>MWp</t>
   </si>
   <si>
-    <t>PV.Profile</t>
-  </si>
-  <si>
-    <t>Clock number</t>
+    <t>PV.Profiel</t>
+  </si>
+  <si>
+    <t>Klokgetal</t>
   </si>
   <si>
     <t>transformer_load_1</t>
   </si>
   <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>2 % per year</t>
+    <t>Industrie</t>
+  </si>
+  <si>
+    <t>2 % per jaar</t>
   </si>
   <si>
     <t>YNyn0</t>
   </si>
   <si>
-    <t>Passive filter</t>
-  </si>
-  <si>
-    <t>Active filter</t>
+    <t>Passief filter</t>
+  </si>
+  <si>
+    <t>Actief filter</t>
   </si>
   <si>
     <t>shunt1</t>
@@ -912,13 +912,13 @@
     <t>7 Ohm</t>
   </si>
   <si>
-    <t>Scaling</t>
+    <t>Schaling</t>
   </si>
   <si>
     <t>‰</t>
   </si>
   <si>
-    <t>Width</t>
+    <t>Breedte</t>
   </si>
   <si>
     <t>° NB</t>
@@ -930,13 +930,13 @@
     <t>Inverter.Snom</t>
   </si>
   <si>
-    <t>Inverter.efficiency type</t>
-  </si>
-  <si>
-    <t>Inverter.P-control</t>
-  </si>
-  <si>
-    <t>Inverter.Q-control</t>
+    <t>Inverter.Rendementtype</t>
+  </si>
+  <si>
+    <t>Inverter.P-regeling</t>
+  </si>
+  <si>
+    <t>Inverter.Q-regeling</t>
   </si>
   <si>
     <t>Inverter.cos phi</t>
@@ -1327,38 +1327,38 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="2" width="6.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="5.88671875" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
-    <col min="13" max="13" width="16.21875" customWidth="1"/>
-    <col min="14" max="14" width="24.21875" customWidth="1"/>
-    <col min="15" max="15" width="22.88671875" customWidth="1"/>
-    <col min="16" max="16" width="23.5546875" customWidth="1"/>
-    <col min="17" max="17" width="26.44140625" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" customWidth="1"/>
-    <col min="19" max="19" width="16" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="23.44140625" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" customWidth="1"/>
+    <col min="16" max="16" width="25.21875" customWidth="1"/>
+    <col min="17" max="17" width="12.21875" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" customWidth="1"/>
+    <col min="19" max="19" width="15.44140625" customWidth="1"/>
     <col min="20" max="20" width="5.88671875" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" customWidth="1"/>
-    <col min="22" max="22" width="10.88671875" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" customWidth="1"/>
-    <col min="24" max="24" width="13.77734375" customWidth="1"/>
-    <col min="25" max="25" width="11.109375" customWidth="1"/>
-    <col min="26" max="26" width="8.77734375" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="13" customWidth="1"/>
+    <col min="23" max="23" width="12" customWidth="1"/>
+    <col min="24" max="24" width="14.109375" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" customWidth="1"/>
+    <col min="26" max="26" width="8.5546875" customWidth="1"/>
     <col min="27" max="28" width="5.88671875" customWidth="1"/>
-    <col min="29" max="29" width="6.33203125" customWidth="1"/>
+    <col min="29" max="29" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
@@ -1789,21 +1789,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
+    <col min="14" max="15" width="5.88671875" customWidth="1"/>
     <col min="16" max="16" width="8.44140625" customWidth="1"/>
     <col min="17" max="17" width="7.77734375" customWidth="1"/>
     <col min="18" max="18" width="8.21875" customWidth="1"/>
@@ -1987,28 +1986,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
     <col min="15" max="15" width="5.88671875" customWidth="1"/>
-    <col min="16" max="16" width="10.21875" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" customWidth="1"/>
     <col min="18" max="18" width="5.88671875" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" customWidth="1"/>
     <col min="20" max="20" width="7.5546875" customWidth="1"/>
     <col min="21" max="21" width="5.88671875" customWidth="1"/>
-    <col min="22" max="22" width="7" customWidth="1"/>
+    <col min="22" max="22" width="7.88671875" customWidth="1"/>
     <col min="23" max="23" width="7.77734375" customWidth="1"/>
     <col min="24" max="24" width="5.88671875" customWidth="1"/>
     <col min="25" max="25" width="6.6640625" customWidth="1"/>
@@ -2018,7 +2017,7 @@
     <col min="29" max="29" width="6.44140625" customWidth="1"/>
     <col min="30" max="30" width="6.109375" customWidth="1"/>
     <col min="31" max="31" width="7" customWidth="1"/>
-    <col min="32" max="32" width="10.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.21875" customWidth="1"/>
     <col min="33" max="33" width="6.21875" customWidth="1"/>
     <col min="34" max="34" width="5.88671875" customWidth="1"/>
     <col min="35" max="35" width="7.77734375" customWidth="1"/>
@@ -2308,28 +2307,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="6.5546875" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
     <col min="16" max="16" width="5.88671875" customWidth="1"/>
     <col min="17" max="17" width="7.77734375" customWidth="1"/>
     <col min="18" max="18" width="20.88671875" customWidth="1"/>
     <col min="19" max="19" width="12.109375" customWidth="1"/>
     <col min="20" max="20" width="6.44140625" customWidth="1"/>
-    <col min="21" max="21" width="9.5546875" customWidth="1"/>
-    <col min="22" max="22" width="13.109375" customWidth="1"/>
+    <col min="21" max="21" width="10.5546875" customWidth="1"/>
+    <col min="22" max="22" width="13.44140625" customWidth="1"/>
     <col min="23" max="23" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2511,31 +2510,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
     <col min="15" max="16" width="5.88671875" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" customWidth="1"/>
-    <col min="18" max="18" width="8.21875" customWidth="1"/>
+    <col min="17" max="17" width="7.77734375" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" customWidth="1"/>
     <col min="19" max="19" width="7.77734375" customWidth="1"/>
-    <col min="20" max="20" width="12.44140625" customWidth="1"/>
+    <col min="20" max="20" width="14.77734375" customWidth="1"/>
     <col min="21" max="22" width="5.88671875" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" customWidth="1"/>
-    <col min="24" max="24" width="18" customWidth="1"/>
-    <col min="25" max="25" width="22.21875" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" customWidth="1"/>
+    <col min="24" max="24" width="18.88671875" customWidth="1"/>
+    <col min="25" max="25" width="19.88671875" customWidth="1"/>
     <col min="26" max="26" width="18.109375" customWidth="1"/>
-    <col min="27" max="27" width="15.21875" customWidth="1"/>
+    <col min="27" max="27" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
@@ -2731,46 +2730,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="20.109375" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" customWidth="1"/>
-    <col min="20" max="20" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" customWidth="1"/>
+    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" customWidth="1"/>
     <col min="21" max="21" width="14.109375" customWidth="1"/>
     <col min="22" max="22" width="19" customWidth="1"/>
     <col min="23" max="23" width="9.77734375" customWidth="1"/>
     <col min="24" max="24" width="10.44140625" customWidth="1"/>
-    <col min="25" max="25" width="18" customWidth="1"/>
-    <col min="26" max="26" width="22.21875" customWidth="1"/>
+    <col min="25" max="25" width="18.88671875" customWidth="1"/>
+    <col min="26" max="26" width="19.88671875" customWidth="1"/>
     <col min="27" max="27" width="18.109375" customWidth="1"/>
-    <col min="28" max="28" width="15.21875" customWidth="1"/>
-    <col min="29" max="30" width="5.88671875" customWidth="1"/>
-    <col min="31" max="31" width="11.109375" customWidth="1"/>
+    <col min="28" max="28" width="19.44140625" customWidth="1"/>
+    <col min="29" max="29" width="10.6640625" customWidth="1"/>
+    <col min="30" max="30" width="5.88671875" customWidth="1"/>
+    <col min="31" max="31" width="10.109375" customWidth="1"/>
     <col min="32" max="32" width="6.21875" customWidth="1"/>
     <col min="33" max="34" width="7.88671875" customWidth="1"/>
     <col min="35" max="37" width="5.88671875" customWidth="1"/>
-    <col min="38" max="38" width="11.88671875" customWidth="1"/>
-    <col min="39" max="39" width="14.33203125" customWidth="1"/>
-    <col min="40" max="40" width="8.88671875" customWidth="1"/>
-    <col min="41" max="41" width="8.5546875" customWidth="1"/>
-    <col min="42" max="42" width="8.6640625" customWidth="1"/>
-    <col min="43" max="43" width="9.33203125" customWidth="1"/>
-    <col min="44" max="44" width="9" customWidth="1"/>
+    <col min="38" max="38" width="11.109375" customWidth="1"/>
+    <col min="39" max="39" width="9.88671875" customWidth="1"/>
+    <col min="40" max="40" width="9.77734375" customWidth="1"/>
+    <col min="41" max="41" width="12.5546875" customWidth="1"/>
+    <col min="42" max="42" width="8.88671875" customWidth="1"/>
+    <col min="43" max="43" width="9.6640625" customWidth="1"/>
+    <col min="44" max="44" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
@@ -3111,25 +3111,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
     <col min="14" max="14" width="5.88671875" customWidth="1"/>
     <col min="15" max="15" width="7.33203125" customWidth="1"/>
     <col min="16" max="16" width="6.6640625" customWidth="1"/>
     <col min="17" max="17" width="7.77734375" customWidth="1"/>
-    <col min="18" max="18" width="13.21875" customWidth="1"/>
-    <col min="19" max="19" width="12.21875" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" customWidth="1"/>
+    <col min="19" max="19" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -3289,19 +3289,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
     <col min="14" max="14" width="5.88671875" customWidth="1"/>
     <col min="15" max="15" width="6.6640625" customWidth="1"/>
     <col min="16" max="16" width="7.77734375" customWidth="1"/>
@@ -3438,19 +3438,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
     <col min="14" max="14" width="7.109375" customWidth="1"/>
     <col min="15" max="16" width="5.88671875" customWidth="1"/>
   </cols>
@@ -3589,29 +3589,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="8.77734375" customWidth="1"/>
     <col min="16" max="16" width="7.77734375" customWidth="1"/>
-    <col min="17" max="17" width="6.77734375" customWidth="1"/>
+    <col min="17" max="17" width="8.5546875" customWidth="1"/>
     <col min="18" max="18" width="7.33203125" customWidth="1"/>
     <col min="19" max="19" width="6.44140625" customWidth="1"/>
     <col min="20" max="20" width="14.88671875" customWidth="1"/>
-    <col min="21" max="21" width="23.77734375" customWidth="1"/>
-    <col min="22" max="22" width="18.33203125" customWidth="1"/>
-    <col min="23" max="23" width="18.77734375" customWidth="1"/>
+    <col min="21" max="21" width="25.21875" customWidth="1"/>
+    <col min="22" max="22" width="19.21875" customWidth="1"/>
+    <col min="23" max="23" width="19.5546875" customWidth="1"/>
     <col min="24" max="24" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3807,15 +3807,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
     <col min="4" max="4" width="9.21875" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" customWidth="1"/>
     <col min="8" max="8" width="5.88671875" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" customWidth="1"/>
     <col min="10" max="10" width="5.88671875" customWidth="1"/>
     <col min="11" max="11" width="6.77734375" customWidth="1"/>
     <col min="12" max="12" width="6.6640625" customWidth="1"/>
@@ -3827,8 +3827,8 @@
     <col min="20" max="20" width="6.5546875" customWidth="1"/>
     <col min="21" max="21" width="5.88671875" customWidth="1"/>
     <col min="22" max="22" width="7.77734375" customWidth="1"/>
-    <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="24" max="24" width="14.21875" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" customWidth="1"/>
+    <col min="24" max="24" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
@@ -4049,24 +4049,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.21875" customWidth="1"/>
     <col min="19" max="19" width="7.33203125" customWidth="1"/>
     <col min="20" max="20" width="6.33203125" customWidth="1"/>
     <col min="21" max="21" width="6.5546875" customWidth="1"/>
@@ -4077,9 +4077,9 @@
     <col min="26" max="26" width="9.6640625" customWidth="1"/>
     <col min="27" max="27" width="8.44140625" customWidth="1"/>
     <col min="28" max="28" width="5.88671875" customWidth="1"/>
-    <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="30" max="30" width="7.5546875" customWidth="1"/>
-    <col min="31" max="31" width="22.88671875" customWidth="1"/>
+    <col min="29" max="29" width="12.88671875" customWidth="1"/>
+    <col min="30" max="30" width="9.21875" customWidth="1"/>
+    <col min="31" max="31" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
@@ -4327,25 +4327,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" customWidth="1"/>
-    <col min="19" max="19" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.21875" customWidth="1"/>
+    <col min="19" max="19" width="18.21875" customWidth="1"/>
     <col min="20" max="21" width="6.109375" customWidth="1"/>
     <col min="22" max="22" width="5.88671875" customWidth="1"/>
     <col min="23" max="24" width="6.109375" customWidth="1"/>
@@ -4565,24 +4565,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.21875" customWidth="1"/>
     <col min="19" max="19" width="5.88671875" customWidth="1"/>
     <col min="20" max="20" width="6.5546875" customWidth="1"/>
   </cols>
@@ -4731,26 +4731,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.21875" customWidth="1"/>
     <col min="19" max="19" width="14.6640625" customWidth="1"/>
-    <col min="20" max="20" width="11.109375" customWidth="1"/>
+    <col min="20" max="20" width="10.109375" customWidth="1"/>
     <col min="21" max="21" width="5.88671875" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" customWidth="1"/>
     <col min="23" max="28" width="5.88671875" customWidth="1"/>
@@ -4984,38 +4984,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" customWidth="1"/>
-    <col min="19" max="19" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.21875" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" customWidth="1"/>
     <col min="20" max="20" width="8.21875" customWidth="1"/>
     <col min="21" max="26" width="5.88671875" customWidth="1"/>
     <col min="27" max="27" width="6.77734375" customWidth="1"/>
-    <col min="28" max="28" width="11.44140625" customWidth="1"/>
-    <col min="29" max="29" width="15.77734375" customWidth="1"/>
-    <col min="30" max="30" width="8" customWidth="1"/>
+    <col min="28" max="28" width="13.109375" customWidth="1"/>
+    <col min="29" max="29" width="10.5546875" customWidth="1"/>
+    <col min="30" max="30" width="9.109375" customWidth="1"/>
     <col min="31" max="31" width="5.88671875" customWidth="1"/>
     <col min="32" max="32" width="7.21875" customWidth="1"/>
     <col min="33" max="34" width="5.88671875" customWidth="1"/>
     <col min="35" max="35" width="6" customWidth="1"/>
     <col min="36" max="36" width="6.44140625" customWidth="1"/>
     <col min="37" max="37" width="22.21875" customWidth="1"/>
-    <col min="38" max="38" width="11.109375" customWidth="1"/>
+    <col min="38" max="38" width="10.109375" customWidth="1"/>
     <col min="39" max="39" width="6.21875" customWidth="1"/>
     <col min="40" max="41" width="7.88671875" customWidth="1"/>
     <col min="42" max="43" width="5.88671875" customWidth="1"/>
@@ -5024,12 +5024,12 @@
     <col min="46" max="46" width="7.33203125" customWidth="1"/>
     <col min="47" max="47" width="6.109375" customWidth="1"/>
     <col min="48" max="48" width="6.5546875" customWidth="1"/>
-    <col min="49" max="49" width="11.88671875" customWidth="1"/>
-    <col min="50" max="50" width="8.88671875" customWidth="1"/>
-    <col min="51" max="51" width="8.5546875" customWidth="1"/>
-    <col min="52" max="52" width="8.6640625" customWidth="1"/>
-    <col min="53" max="53" width="9.33203125" customWidth="1"/>
-    <col min="54" max="54" width="9" customWidth="1"/>
+    <col min="49" max="49" width="11.109375" customWidth="1"/>
+    <col min="50" max="50" width="9.77734375" customWidth="1"/>
+    <col min="51" max="51" width="12.5546875" customWidth="1"/>
+    <col min="52" max="52" width="8.88671875" customWidth="1"/>
+    <col min="53" max="53" width="9.6640625" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.3">
@@ -5435,35 +5435,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" customWidth="1"/>
-    <col min="19" max="19" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.21875" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" customWidth="1"/>
     <col min="20" max="20" width="6.77734375" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" customWidth="1"/>
-    <col min="22" max="22" width="15.77734375" customWidth="1"/>
-    <col min="23" max="23" width="8" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" customWidth="1"/>
+    <col min="22" max="22" width="10.5546875" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" customWidth="1"/>
     <col min="24" max="24" width="5.88671875" customWidth="1"/>
     <col min="25" max="25" width="7.21875" customWidth="1"/>
     <col min="26" max="27" width="5.88671875" customWidth="1"/>
     <col min="28" max="28" width="29.109375" customWidth="1"/>
     <col min="29" max="29" width="8.21875" customWidth="1"/>
-    <col min="30" max="30" width="11.109375" customWidth="1"/>
+    <col min="30" max="30" width="10.109375" customWidth="1"/>
     <col min="31" max="31" width="6.21875" customWidth="1"/>
     <col min="32" max="33" width="7.88671875" customWidth="1"/>
     <col min="34" max="34" width="6.88671875" customWidth="1"/>
@@ -5475,11 +5475,11 @@
     <col min="40" max="42" width="5.88671875" customWidth="1"/>
     <col min="43" max="43" width="6.109375" customWidth="1"/>
     <col min="44" max="44" width="6.5546875" customWidth="1"/>
-    <col min="45" max="45" width="8.88671875" customWidth="1"/>
-    <col min="46" max="46" width="8.5546875" customWidth="1"/>
-    <col min="47" max="47" width="8.6640625" customWidth="1"/>
-    <col min="48" max="48" width="9.33203125" customWidth="1"/>
-    <col min="49" max="49" width="9" customWidth="1"/>
+    <col min="45" max="45" width="9.77734375" customWidth="1"/>
+    <col min="46" max="46" width="12.5546875" customWidth="1"/>
+    <col min="47" max="47" width="8.88671875" customWidth="1"/>
+    <col min="48" max="48" width="9.6640625" customWidth="1"/>
+    <col min="49" max="49" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.3">
@@ -5873,55 +5873,56 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" customWidth="1"/>
-    <col min="18" max="18" width="14.5546875" customWidth="1"/>
-    <col min="19" max="19" width="17.88671875" customWidth="1"/>
-    <col min="20" max="20" width="16.21875" customWidth="1"/>
-    <col min="21" max="21" width="24.21875" customWidth="1"/>
-    <col min="22" max="22" width="22.88671875" customWidth="1"/>
-    <col min="23" max="23" width="23.5546875" customWidth="1"/>
-    <col min="24" max="24" width="5.88671875" customWidth="1"/>
-    <col min="25" max="25" width="6" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" customWidth="1"/>
+    <col min="16" max="16" width="15.77734375" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="15.109375" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" customWidth="1"/>
+    <col min="22" max="22" width="17.6640625" customWidth="1"/>
+    <col min="23" max="23" width="25.21875" customWidth="1"/>
+    <col min="24" max="24" width="12.44140625" customWidth="1"/>
+    <col min="25" max="25" width="11.77734375" customWidth="1"/>
     <col min="26" max="34" width="5.88671875" customWidth="1"/>
     <col min="35" max="37" width="8" customWidth="1"/>
-    <col min="38" max="39" width="14.44140625" customWidth="1"/>
-    <col min="40" max="40" width="15.77734375" customWidth="1"/>
-    <col min="41" max="41" width="8" customWidth="1"/>
+    <col min="38" max="39" width="15.5546875" customWidth="1"/>
+    <col min="40" max="40" width="10.5546875" customWidth="1"/>
+    <col min="41" max="41" width="9.109375" customWidth="1"/>
     <col min="42" max="42" width="5.88671875" customWidth="1"/>
     <col min="43" max="43" width="7.21875" customWidth="1"/>
     <col min="44" max="46" width="5.88671875" customWidth="1"/>
     <col min="47" max="49" width="7.44140625" customWidth="1"/>
     <col min="50" max="52" width="7.88671875" customWidth="1"/>
     <col min="53" max="58" width="5.88671875" customWidth="1"/>
-    <col min="59" max="61" width="6.21875" customWidth="1"/>
+    <col min="59" max="61" width="6.6640625" customWidth="1"/>
     <col min="62" max="69" width="5.88671875" customWidth="1"/>
     <col min="70" max="72" width="7.21875" customWidth="1"/>
-    <col min="73" max="73" width="11.88671875" customWidth="1"/>
-    <col min="74" max="74" width="10.33203125" customWidth="1"/>
-    <col min="75" max="75" width="10" customWidth="1"/>
-    <col min="76" max="76" width="10.109375" customWidth="1"/>
-    <col min="77" max="77" width="10.88671875" customWidth="1"/>
-    <col min="78" max="79" width="10.5546875" customWidth="1"/>
-    <col min="80" max="80" width="10.21875" customWidth="1"/>
-    <col min="81" max="81" width="10.33203125" customWidth="1"/>
-    <col min="82" max="82" width="11" customWidth="1"/>
-    <col min="83" max="83" width="10.77734375" customWidth="1"/>
+    <col min="73" max="73" width="11.109375" customWidth="1"/>
+    <col min="74" max="74" width="11.5546875" customWidth="1"/>
+    <col min="75" max="75" width="14.33203125" customWidth="1"/>
+    <col min="76" max="76" width="10.77734375" customWidth="1"/>
+    <col min="77" max="77" width="11.44140625" customWidth="1"/>
+    <col min="78" max="78" width="11.109375" customWidth="1"/>
+    <col min="79" max="79" width="10.88671875" customWidth="1"/>
+    <col min="80" max="80" width="13.6640625" customWidth="1"/>
+    <col min="81" max="81" width="10.109375" customWidth="1"/>
+    <col min="82" max="82" width="10.77734375" customWidth="1"/>
+    <col min="83" max="83" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:83" x14ac:dyDescent="0.3">

</xml_diff>